<commit_message>
hasta aca estamos perfecto, sin errores, actualizacion de tablas y ajustes
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -46,7 +46,7 @@
     <t>Bruno Díaz</t>
   </si>
   <si>
-    <t>12345678A</t>
+    <t>12345678A2</t>
   </si>
   <si>
     <t>98765432B</t>
@@ -58,13 +58,13 @@
     <t>bruno@example.com</t>
   </si>
   <si>
-    <t>600111222</t>
-  </si>
-  <si>
-    <t>600333444</t>
-  </si>
-  <si>
-    <t>Calle Sol</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>678678</t>
+  </si>
+  <si>
+    <t>Calle Sol78</t>
   </si>
   <si>
     <t>Av. Luna 45</t>

</xml_diff>